<commit_message>
Fixed Address geocode excel conversion
</commit_message>
<xml_diff>
--- a/drive-time-locator/Backend/locations_with_coords.xlsx
+++ b/drive-time-locator/Backend/locations_with_coords.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>555 Robson St</t>
+          <t>555 Robson St, VANCOUVER, BC, V6B 1A6</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -496,7 +496,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4601 Westway Park Boulevard</t>
+          <t>4601 Westway Park Boulevard, Houston, TX, 77041</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -519,14 +519,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>#3 CALLE ACACIA OFICINA 201-B</t>
+          <t>#3 CALLE ACACIA OFICINA 201-B, SAN JUAN, PR, 920</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>25.826598</v>
+        <v>18.46633</v>
       </c>
       <c r="E4" t="n">
-        <v>-108.995069</v>
+        <v>-66.10572000000001</v>
       </c>
     </row>
     <row r="5">
@@ -542,7 +542,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>171 AUHANA RD</t>
+          <t>171 AUHANA RD, KIHEI, HI, 96753</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,7 +565,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>98-723 KUAHAO PL STE A13</t>
+          <t>98-723 KUAHAO PL STE A13, PEARL CITY, HI, 96782</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -588,14 +588,14 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>16-711 MILO ST UNIT B</t>
+          <t>16-711 MILO ST UNIT B, KEAAU, HI, 96749</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>64.80244999999999</v>
+        <v>19.627332</v>
       </c>
       <c r="E7" t="n">
-        <v>-147.450512</v>
+        <v>-155.030647</v>
       </c>
     </row>
     <row r="8">
@@ -611,14 +611,14 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3989 1ST ST STE E</t>
+          <t>3989 1ST ST STE E, LIVERMORE, CA, 94551</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>37.645259</v>
+        <v>37.6781</v>
       </c>
       <c r="E8" t="n">
-        <v>-98.43555499999999</v>
+        <v>-121.784928</v>
       </c>
     </row>
     <row r="9">
@@ -634,7 +634,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10604 N PALISADES WAY</t>
+          <t>10604 N PALISADES WAY, BOISE, ID, 83714</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -657,14 +657,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6344 US RT 22-3</t>
+          <t>6344 US RT 22-3, MORROW, OH, 45152</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>44.141366</v>
+        <v>40.509237</v>
       </c>
       <c r="E10" t="n">
-        <v>-72.31336899999999</v>
+        <v>-82.79409699999999</v>
       </c>
     </row>
     <row r="11">
@@ -680,7 +680,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1725 N PACKER RD</t>
+          <t>1725 N PACKER RD, SPRINGFIELD, MO, 65803</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -703,7 +703,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>932 KENMORE AVE</t>
+          <t>932 KENMORE AVE, BUFFALO, NY, 14216-1462</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -726,14 +726,14 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5510 N. HWY 27</t>
+          <t>5510 N. HWY 27, BRYANT, IN, 47326-8835</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>34.834315</v>
+        <v>35.74174</v>
       </c>
       <c r="E13" t="n">
-        <v>-85.24355300000001</v>
+        <v>-91.65208</v>
       </c>
     </row>
     <row r="14">
@@ -749,14 +749,14 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7511 KEKAA ST</t>
+          <t>7511 KEKAA ST, HONOLULU, HI, 96825-2805</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>21.296473</v>
+        <v>21.40572</v>
       </c>
       <c r="E14" t="n">
-        <v>-157.674734</v>
+        <v>-157.789396</v>
       </c>
     </row>
     <row r="15">
@@ -772,7 +772,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>3260 OLD FARM LN</t>
+          <t>3260 OLD FARM LN, COMMERCE, MI, 48390</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -795,14 +795,14 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>6150 W CHANDLER BLVD #17</t>
+          <t>6150 W CHANDLER BLVD #17, CHANDLER, AZ, 85226</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>33.305405</v>
+        <v>33.310045</v>
       </c>
       <c r="E16" t="n">
-        <v>-111.909034</v>
+        <v>-111.861363</v>
       </c>
     </row>
     <row r="17">
@@ -818,7 +818,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>680 Redna Terrace</t>
+          <t>680 Redna Terrace, Cincinnati, OH, 45215</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -841,14 +841,14 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>91-6221 KAPOLEI PARKWAY UNIT 11</t>
+          <t>91-6221 KAPOLEI PARKWAY UNIT 11, EWA BEACH, HI, 96706</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>21.335959</v>
+        <v>21.325072</v>
       </c>
       <c r="E18" t="n">
-        <v>-158.053795</v>
+        <v>-158.028212</v>
       </c>
     </row>
     <row r="19">
@@ -864,7 +864,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>35 OWOSSO DR</t>
+          <t>35 OWOSSO DR, EUGENE, OR, 97404-2628</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -887,14 +887,14 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14500 ROSCOE BLVD 4TH FLOOR</t>
+          <t>14500 ROSCOE BLVD 4TH FLOOR, PANORAMA CITY, CA, 91402</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>34.221579</v>
+        <v>34.221238</v>
       </c>
       <c r="E20" t="n">
-        <v>-118.376369</v>
+        <v>-118.444706</v>
       </c>
     </row>
     <row r="21">
@@ -910,14 +910,14 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>127 W MAIN ST APT A</t>
+          <t>127 W MAIN ST APT A, JACKSON, MO, 63755-1879</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>46.563824</v>
+        <v>37.383607</v>
       </c>
       <c r="E21" t="n">
-        <v>-112.435421</v>
+        <v>-89.67747900000001</v>
       </c>
     </row>
     <row r="22">
@@ -933,14 +933,14 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>132 TERRACE DR</t>
+          <t>132 TERRACE DR, INDEPENDENCE, IA, 50644</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>36.889074</v>
+        <v>42.467132</v>
       </c>
       <c r="E22" t="n">
-        <v>-89.575926</v>
+        <v>-91.878241</v>
       </c>
     </row>
     <row r="23">
@@ -956,14 +956,14 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>535 PINE ST</t>
+          <t>535 PINE ST, CENTRAL FALLS, RI, 2863</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>39.135353</v>
+        <v>41.884462</v>
       </c>
       <c r="E23" t="n">
-        <v>-95.95522800000001</v>
+        <v>-71.39638100000001</v>
       </c>
     </row>
     <row r="24">
@@ -979,14 +979,14 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>6210 CARDWELL RD</t>
+          <t>6210 CARDWELL RD, CORRYTON, TN, 37721-3715</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>36.926368</v>
+        <v>36.15369</v>
       </c>
       <c r="E24" t="n">
-        <v>-87.181316</v>
+        <v>-83.78241</v>
       </c>
     </row>
     <row r="25">
@@ -1002,14 +1002,14 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>801 PRESSLEY RD STE 100-C</t>
+          <t>801 PRESSLEY RD STE 100-C, CHARLOTTE, NC, 28217</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>35.600409</v>
+        <v>35.188483</v>
       </c>
       <c r="E25" t="n">
-        <v>-82.508619</v>
+        <v>-80.893687</v>
       </c>
     </row>
     <row r="26">
@@ -1025,7 +1025,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>12914 SE 257TH ST</t>
+          <t>12914 SE 257TH ST, KENT, WA, 98030</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1048,14 +1048,14 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>4363 BURTON LN</t>
+          <t>4363 BURTON LN, NORTH GARDEN, VA, 22959</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>32.096141</v>
+        <v>37.9407</v>
       </c>
       <c r="E27" t="n">
-        <v>-90.16226899999999</v>
+        <v>-78.63668</v>
       </c>
     </row>
     <row r="28">
@@ -1071,14 +1071,14 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>10415 HARMON RD</t>
+          <t>10415 HARMON RD, BERLIN HEIGHTS, OH, 44814</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>36.529843</v>
+        <v>41.323565</v>
       </c>
       <c r="E28" t="n">
-        <v>-88.267402</v>
+        <v>-82.49020899999999</v>
       </c>
     </row>
     <row r="29">
@@ -1094,14 +1094,14 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>841 WATSON LN W</t>
+          <t>841 WATSON LN W, NEW BRAUNFELS, TX, 78130</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>29.787388</v>
+        <v>29.694703</v>
       </c>
       <c r="E29" t="n">
-        <v>-98.04325300000001</v>
+        <v>-98.116089</v>
       </c>
     </row>
     <row r="30">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>903 S DEER RUN</t>
+          <t>903 S DEER RUN, ELLETTSVILLE, IN, 47429</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>7735 WINTON DR</t>
+          <t>7735 WINTON DR, INDIANAPOLIS, IN, 46268</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1163,14 +1163,14 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>9285 UPSTREAM LN</t>
+          <t>9285 UPSTREAM LN, KNOXVILLE, TN, 37931</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>38.505677</v>
+        <v>35.973011</v>
       </c>
       <c r="E32" t="n">
-        <v>-79.054361</v>
+        <v>-83.969472</v>
       </c>
     </row>
     <row r="33">
@@ -1186,14 +1186,14 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>930 BONNIE LN</t>
+          <t>930 BONNIE LN, AUBURN, CA, 95603-9452</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>41.527285</v>
+        <v>38.898076</v>
       </c>
       <c r="E33" t="n">
-        <v>-81.448522</v>
+        <v>-121.071247</v>
       </c>
     </row>
     <row r="34">
@@ -1209,14 +1209,14 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>138 STERLING AVE</t>
+          <t>138 STERLING AVE, RITTMAN, OH, 44270-1655</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>49.833646</v>
+        <v>40.966545</v>
       </c>
       <c r="E34" t="n">
-        <v>-97.10127300000001</v>
+        <v>-81.788777</v>
       </c>
     </row>
     <row r="35">
@@ -1232,14 +1232,14 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>180 GRANTON EDGE LN</t>
+          <t>180 GRANTON EDGE LN, SUMMERVILLE, SC, 29486</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>33.144226</v>
+        <v>33.012176</v>
       </c>
       <c r="E35" t="n">
-        <v>-80.093373</v>
+        <v>-80.182766</v>
       </c>
     </row>
     <row r="36">
@@ -1255,14 +1255,14 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>9756 TALL TIMBER DR</t>
+          <t>9756 TALL TIMBER DR, WEST CHESTER, OH, 45241-1221</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>42.089501</v>
+        <v>39.306282</v>
       </c>
       <c r="E36" t="n">
-        <v>-72.448956</v>
+        <v>-84.381606</v>
       </c>
     </row>
     <row r="37">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>5908 TRIANGLE DR</t>
+          <t>5908 TRIANGLE DR, RALEIGH, NC, 27617</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1301,14 +1301,14 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1132 E MARKET ST BAY 5</t>
+          <t>1132 E MARKET ST BAY 5, CHARLOTTESVILLE, VA, 22902-5351</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>42.280665</v>
+        <v>38.036141</v>
       </c>
       <c r="E38" t="n">
-        <v>-94.290148</v>
+        <v>-78.48236900000001</v>
       </c>
     </row>
     <row r="39">
@@ -1324,14 +1324,14 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>926 E CHURCH ST</t>
+          <t>926 E CHURCH ST, SANDWICH, IL, 60548</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>41.690599</v>
+        <v>41.644714</v>
       </c>
       <c r="E39" t="n">
-        <v>-94.361904</v>
+        <v>-88.616303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>